<commit_message>
cambios generales salon de la fama e instalaciones
</commit_message>
<xml_diff>
--- a/assets/db/medallistas_uaq.xlsx
+++ b/assets/db/medallistas_uaq.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ordaz\Local Sites\deportesuaq\app\public\wp-content\themes\Deportes-UAQ\assets\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Local Sites\deportes-uaq\app\public\wp-content\themes\Deportes-UAQ\assets\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630C8EBC-5DE6-4BB9-A0C8-B16436A61CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C24A3AD-5A0A-4902-B373-E8822B3D80CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="15" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="15" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="t_un_2001_v" sheetId="1" r:id="rId1"/>
@@ -858,7 +858,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -889,6 +889,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -943,10 +951,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1006,8 +1015,12 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1317,19 +1330,19 @@
       <selection activeCell="H2" sqref="H2:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.88671875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1355,7 +1368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1381,7 +1394,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1407,7 +1420,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1433,7 +1446,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1459,7 +1472,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1485,7 +1498,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1511,7 +1524,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1537,7 +1550,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1563,7 +1576,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1605,18 +1618,18 @@
       <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.88671875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1642,7 +1655,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1668,7 +1681,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1694,7 +1707,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1720,7 +1733,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1746,7 +1759,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1772,7 +1785,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1814,18 +1827,18 @@
       <selection activeCell="H2" sqref="H2:H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.88671875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1851,7 +1864,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1877,7 +1890,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1903,7 +1916,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1945,18 +1958,18 @@
       <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.88671875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1982,7 +1995,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2008,7 +2021,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2034,7 +2047,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2060,7 +2073,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2086,7 +2099,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2112,7 +2125,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2154,19 +2167,19 @@
       <selection activeCell="H2" sqref="H2:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.88671875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2192,7 +2205,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2218,7 +2231,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2244,7 +2257,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2270,7 +2283,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2296,7 +2309,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2322,7 +2335,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2348,7 +2361,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2390,19 +2403,19 @@
       <selection activeCell="H2" sqref="H2:H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.88671875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2428,7 +2441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2454,7 +2467,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2480,7 +2493,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2506,7 +2519,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2532,7 +2545,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2558,7 +2571,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2584,7 +2597,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2610,7 +2623,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2636,7 +2649,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -2662,7 +2675,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2688,7 +2701,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2714,7 +2727,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2756,18 +2769,18 @@
       <selection activeCell="H2" sqref="H2:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.109375" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2793,7 +2806,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2819,7 +2832,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2845,7 +2858,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2871,7 +2884,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2897,7 +2910,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2923,7 +2936,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2949,7 +2962,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2975,7 +2988,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -3001,7 +3014,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -3043,18 +3056,18 @@
       <selection activeCell="H2" sqref="H2:H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.109375" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3080,7 +3093,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -3106,7 +3119,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -3132,7 +3145,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -3158,7 +3171,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -3184,7 +3197,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -3210,7 +3223,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -3236,7 +3249,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -3262,7 +3275,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -3304,19 +3317,19 @@
       <selection activeCell="I2" sqref="I2:I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.44140625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>52</v>
       </c>
@@ -3345,7 +3358,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>3</v>
       </c>
@@ -3374,7 +3387,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>4</v>
       </c>
@@ -3403,7 +3416,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>5</v>
       </c>
@@ -3432,7 +3445,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>6</v>
       </c>
@@ -3461,7 +3474,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>7</v>
       </c>
@@ -3490,7 +3503,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>8</v>
       </c>
@@ -3535,19 +3548,19 @@
       <selection activeCell="I2" sqref="I2:I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.88671875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>52</v>
       </c>
@@ -3576,7 +3589,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>2</v>
       </c>
@@ -3605,7 +3618,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>3</v>
       </c>
@@ -3634,7 +3647,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>4</v>
       </c>
@@ -3663,7 +3676,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>5</v>
       </c>
@@ -3692,7 +3705,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>6</v>
       </c>
@@ -3721,7 +3734,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>7</v>
       </c>
@@ -3750,7 +3763,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>8</v>
       </c>
@@ -3779,7 +3792,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>9</v>
       </c>
@@ -3808,7 +3821,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>10</v>
       </c>
@@ -3837,7 +3850,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>11</v>
       </c>
@@ -3866,7 +3879,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>12</v>
       </c>
@@ -3895,7 +3908,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>13</v>
       </c>
@@ -3936,23 +3949,23 @@
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="62.77734375" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3978,7 +3991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -4000,11 +4013,11 @@
       <c r="G2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="21" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -4027,10 +4040,10 @@
         <v>20</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -4056,7 +4069,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -4082,7 +4095,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -4108,7 +4121,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -4134,7 +4147,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -4161,6 +4174,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{CA3CDFB3-D92A-457B-B110-E0E6D9C09456}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4176,19 +4192,19 @@
       <selection activeCell="H2" sqref="H2:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.88671875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4214,7 +4230,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -4240,7 +4256,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -4266,7 +4282,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -4292,7 +4308,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -4318,7 +4334,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -4344,7 +4360,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -4370,7 +4386,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -4396,7 +4412,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -4422,7 +4438,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18">
         <v>9</v>
       </c>
@@ -4460,23 +4476,23 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="69.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="74.21875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4502,7 +4518,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -4528,7 +4544,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -4550,11 +4566,11 @@
       <c r="G3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="21" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -4576,11 +4592,11 @@
       <c r="G4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="21" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -4606,7 +4622,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -4632,7 +4648,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -4659,6 +4675,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{F6826919-3754-4568-8AF6-EB2D59359785}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{CA866113-62F3-47CC-B7D9-4E6714EFC970}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4674,19 +4694,19 @@
       <selection activeCell="H2" sqref="H2:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.88671875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4712,7 +4732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -4738,7 +4758,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -4764,7 +4784,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -4790,7 +4810,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -4816,7 +4836,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -4842,7 +4862,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -4868,7 +4888,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -4894,7 +4914,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -4920,7 +4940,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -4946,7 +4966,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -4988,19 +5008,19 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.88671875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5026,7 +5046,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -5052,35 +5072,35 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
       <c r="H3" s="15"/>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="H6" s="15"/>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="H8" s="15"/>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="H9" s="15"/>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="H10" s="15"/>
     </row>
@@ -5100,19 +5120,19 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.88671875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5138,7 +5158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -5180,19 +5200,19 @@
       <selection activeCell="H2" sqref="H2:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.88671875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5218,7 +5238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -5244,7 +5264,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -5270,7 +5290,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -5296,7 +5316,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -5322,7 +5342,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -5364,19 +5384,19 @@
       <selection activeCell="H2" sqref="H2:H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.88671875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5402,7 +5422,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -5428,7 +5448,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -5454,7 +5474,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -5480,7 +5500,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -5506,7 +5526,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -5532,7 +5552,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -5558,7 +5578,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -5584,7 +5604,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -5610,7 +5630,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -5636,7 +5656,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -5662,7 +5682,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -5688,7 +5708,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -5714,7 +5734,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -5740,7 +5760,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -5766,7 +5786,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -5792,7 +5812,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -5818,7 +5838,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -5844,7 +5864,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -5870,7 +5890,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -5896,7 +5916,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -5922,7 +5942,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -5964,18 +5984,18 @@
       <selection activeCell="H2" sqref="H2:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.88671875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6001,7 +6021,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -6027,7 +6047,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -6053,7 +6073,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -6079,7 +6099,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -6105,7 +6125,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -6147,18 +6167,18 @@
       <selection activeCell="H2" sqref="H2:H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.88671875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6184,7 +6204,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -6210,7 +6230,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -6236,7 +6256,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -6262,7 +6282,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -6288,7 +6308,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -6314,7 +6334,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -6340,7 +6360,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -6366,7 +6386,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>

</xml_diff>